<commit_message>
PDF merge code edited with change
</commit_message>
<xml_diff>
--- a/DDSM/PDF Mearge/BL_Invoice.xlsx
+++ b/DDSM/PDF Mearge/BL_Invoice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssc.achauhan\Desktop\Projects\DDSM\PDF Mearge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CF599B-D17E-483C-AEF7-D25EC6689A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6C1921-AF85-434A-8A47-6C6C63297448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Combining_PDF" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Combining_PDF!$A$1:$C$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Combining_PDF!$A$1:$C$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Invoice_Number</t>
   </si>
@@ -44,34 +44,187 @@
     <t>Combined_Name</t>
   </si>
   <si>
-    <t>BL_Number</t>
-  </si>
-  <si>
-    <t>NAOB0038407</t>
-  </si>
-  <si>
-    <t>NAOB0038411</t>
-  </si>
-  <si>
-    <t>NAOB0038412</t>
-  </si>
-  <si>
-    <t>SGN1631471</t>
-  </si>
-  <si>
-    <t>SGN1646460</t>
-  </si>
-  <si>
-    <t>SGN1646464</t>
-  </si>
-  <si>
-    <t>NAOB0038407-SGN1631471</t>
-  </si>
-  <si>
-    <t>NAOB0038411-SGN1646460</t>
-  </si>
-  <si>
-    <t>NAOB0038412-SGN1646464</t>
+    <t>BL Number</t>
+  </si>
+  <si>
+    <t>NAIM9803074</t>
+  </si>
+  <si>
+    <t>NAIM9803075</t>
+  </si>
+  <si>
+    <t>NAIM9803076</t>
+  </si>
+  <si>
+    <t>NAIM9803077</t>
+  </si>
+  <si>
+    <t>NAIM9803079</t>
+  </si>
+  <si>
+    <t>NAIM9803080</t>
+  </si>
+  <si>
+    <t>NAIM9803081</t>
+  </si>
+  <si>
+    <t>NAIM9803082</t>
+  </si>
+  <si>
+    <t>NAIM9803083</t>
+  </si>
+  <si>
+    <t>NAIM9803085</t>
+  </si>
+  <si>
+    <t>NAIM9803086</t>
+  </si>
+  <si>
+    <t>NAIM9803220</t>
+  </si>
+  <si>
+    <t>NAIM9803221</t>
+  </si>
+  <si>
+    <t>NAIM9803222</t>
+  </si>
+  <si>
+    <t>NAIM9803223</t>
+  </si>
+  <si>
+    <t>NAIM9803224</t>
+  </si>
+  <si>
+    <t>NAIM9803225</t>
+  </si>
+  <si>
+    <t>NAIM9803226</t>
+  </si>
+  <si>
+    <t>NAIM9803233</t>
+  </si>
+  <si>
+    <t>NAIM9803238</t>
+  </si>
+  <si>
+    <t>YAGA003514</t>
+  </si>
+  <si>
+    <t>YAGA003515</t>
+  </si>
+  <si>
+    <t>YAGA003516</t>
+  </si>
+  <si>
+    <t>YAGA003539</t>
+  </si>
+  <si>
+    <t>YGPV142368</t>
+  </si>
+  <si>
+    <t>YGPV142434</t>
+  </si>
+  <si>
+    <t>YGPV142541</t>
+  </si>
+  <si>
+    <t>ZSN0509626</t>
+  </si>
+  <si>
+    <t>ZSN0512123</t>
+  </si>
+  <si>
+    <t>ZSN0516150</t>
+  </si>
+  <si>
+    <t>ZSN0516823</t>
+  </si>
+  <si>
+    <t>ZSN0516829</t>
+  </si>
+  <si>
+    <t>ZSN0516831</t>
+  </si>
+  <si>
+    <t>ZSN0517537</t>
+  </si>
+  <si>
+    <t>ZSN0517705</t>
+  </si>
+  <si>
+    <t>ZSN0517708</t>
+  </si>
+  <si>
+    <t>ZSN0517786</t>
+  </si>
+  <si>
+    <t>ZSN0518753</t>
+  </si>
+  <si>
+    <t>ZSN0520402</t>
+  </si>
+  <si>
+    <t>ZSN0521420</t>
+  </si>
+  <si>
+    <t>NAIM9803074_YAGA003514</t>
+  </si>
+  <si>
+    <t>NAIM9803075_YAGA003515</t>
+  </si>
+  <si>
+    <t>NAIM9803076_YAGA003516</t>
+  </si>
+  <si>
+    <t>NAIM9803077_YAGA003539</t>
+  </si>
+  <si>
+    <t>NAIM9803079_YGPV142368</t>
+  </si>
+  <si>
+    <t>NAIM9803080_YGPV142434</t>
+  </si>
+  <si>
+    <t>NAIM9803081_YGPV142541</t>
+  </si>
+  <si>
+    <t>NAIM9803082_ZSN0509626</t>
+  </si>
+  <si>
+    <t>NAIM9803083_ZSN0512123</t>
+  </si>
+  <si>
+    <t>NAIM9803085_ZSN0516150</t>
+  </si>
+  <si>
+    <t>NAIM9803086_ZSN0516823</t>
+  </si>
+  <si>
+    <t>NAIM9803220_ZSN0516829</t>
+  </si>
+  <si>
+    <t>NAIM9803221_ZSN0516831</t>
+  </si>
+  <si>
+    <t>NAIM9803222_ZSN0517537</t>
+  </si>
+  <si>
+    <t>NAIM9803223_ZSN0517705</t>
+  </si>
+  <si>
+    <t>NAIM9803224_ZSN0517708</t>
+  </si>
+  <si>
+    <t>NAIM9803225_ZSN0517786</t>
+  </si>
+  <si>
+    <t>NAIM9803226_ZSN0518753</t>
+  </si>
+  <si>
+    <t>NAIM9803233_ZSN0520402</t>
+  </si>
+  <si>
+    <t>NAIM9803238_ZSN0521420</t>
   </si>
 </sst>
 </file>
@@ -128,9 +281,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -413,68 +565,247 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>